<commit_message>
Initial Commit of Code and other files
</commit_message>
<xml_diff>
--- a/midiKeyboard BOM.xlsx
+++ b/midiKeyboard BOM.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8149518A-DD4F-4986-BFD2-54C2E67322D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B132DD0D-7EB1-42DC-B063-F62B26D3445D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t xml:space="preserve">Item </t>
   </si>
@@ -69,27 +69,9 @@
     <t>LIon Battery</t>
   </si>
   <si>
-    <t>Tack Switches</t>
-  </si>
-  <si>
-    <t>Mini Tack Switches</t>
-  </si>
-  <si>
     <t>RGB LED 3mm</t>
   </si>
   <si>
-    <t>NinjaFlex Black</t>
-  </si>
-  <si>
-    <t>NinjaFlex Grey</t>
-  </si>
-  <si>
-    <t>PLA Yellow</t>
-  </si>
-  <si>
-    <t>PLA Black</t>
-  </si>
-  <si>
     <t>Custom PCB</t>
   </si>
   <si>
@@ -100,6 +82,69 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Switch Cap, 9x9, Black</t>
+  </si>
+  <si>
+    <t>653-B32-1210</t>
+  </si>
+  <si>
+    <t>Switch Cap, 9x9, White</t>
+  </si>
+  <si>
+    <t>653-B32-1260</t>
+  </si>
+  <si>
+    <t>Switch Cap, 4x4, Red</t>
+  </si>
+  <si>
+    <t>653-B32-1080</t>
+  </si>
+  <si>
+    <t>Switch Cap, 4x4, Orange</t>
+  </si>
+  <si>
+    <t>Switch Cap, 4x4, Blue</t>
+  </si>
+  <si>
+    <t>653-B32-1020</t>
+  </si>
+  <si>
+    <t>653-B32-1040</t>
+  </si>
+  <si>
+    <t>Tack Switch, plunger, 12x12</t>
+  </si>
+  <si>
+    <t>653-B3W4005S</t>
+  </si>
+  <si>
+    <t>MCP23017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">579-MCP23017-E/SP </t>
+  </si>
+  <si>
+    <t>Interface expander, 16 I/O ports</t>
+  </si>
+  <si>
+    <t>Acrylic Plastic</t>
+  </si>
+  <si>
+    <t>Tack Switch, plunger, 6x6</t>
+  </si>
+  <si>
+    <t>653-B3W1100S</t>
+  </si>
+  <si>
+    <t>Tack On-Off Switch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">653-B3AL-1003P-MS </t>
+  </si>
+  <si>
+    <t>604-WP154A4SUREQBFZG</t>
   </si>
 </sst>
 </file>
@@ -146,7 +191,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -161,6 +206,21 @@
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -442,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,7 +513,7 @@
     <col min="1" max="1" width="22.7109375" style="7" customWidth="1"/>
     <col min="3" max="3" width="21.42578125" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="3"/>
     <col min="7" max="7" width="9" style="5"/>
     <col min="8" max="8" width="9" style="3"/>
@@ -486,162 +546,336 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="9">
         <v>2829</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="12">
         <v>29.95</v>
       </c>
-      <c r="G2" s="5">
-        <v>1</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="G2" s="13">
+        <v>1</v>
+      </c>
+      <c r="H2" s="12">
         <f>F2*G2</f>
         <v>29.95</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="9">
         <v>1578</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="12">
         <v>7.95</v>
       </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ref="H3:H18" si="0">F3*G3</f>
+      <c r="G3" s="13">
+        <v>1</v>
+      </c>
+      <c r="H3" s="12">
+        <f t="shared" ref="H3:H15" si="0">F3*G3</f>
         <v>7.95</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0.69</v>
+      </c>
+      <c r="G4" s="13">
+        <v>20</v>
+      </c>
+      <c r="H4" s="12">
+        <f t="shared" si="0"/>
+        <v>13.799999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.64</v>
+      </c>
+      <c r="G5" s="13">
+        <v>4</v>
+      </c>
+      <c r="H5" s="12">
+        <f t="shared" si="0"/>
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="12">
+        <v>1.79</v>
+      </c>
+      <c r="G6" s="13">
+        <v>1</v>
+      </c>
+      <c r="H6" s="12">
+        <f t="shared" si="0"/>
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G7" s="13">
+        <v>8</v>
+      </c>
+      <c r="H7" s="12">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G8" s="13">
+        <v>12</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="0"/>
+        <v>3.3600000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.25</v>
+      </c>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
+      <c r="H9" s="12">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="12">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
+      <c r="H10" s="12">
+        <f t="shared" si="0"/>
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G11" s="13">
+        <v>1</v>
+      </c>
+      <c r="H11" s="12">
+        <f t="shared" si="0"/>
+        <v>0.28000000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="5">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="B12" s="11"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="12">
+        <v>1.53</v>
+      </c>
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12">
+        <f t="shared" si="0"/>
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="12">
+        <v>1.23</v>
+      </c>
+      <c r="G13" s="13">
+        <v>1</v>
+      </c>
+      <c r="H13" s="12">
+        <f t="shared" si="0"/>
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="12">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="5">
-        <v>4</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="G14" s="13">
+        <v>1</v>
+      </c>
+      <c r="H14" s="12">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="5">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="D15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="E15" s="9"/>
+      <c r="F15" s="12">
+        <v>100</v>
+      </c>
+      <c r="G15" s="13">
+        <v>1</v>
+      </c>
+      <c r="H15" s="12">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G17" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="3">
-        <v>100</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="3">
-        <f>SUM(H2:H11)</f>
-        <v>137.9</v>
+      <c r="H17" s="3">
+        <f>SUM(H2:H15)</f>
+        <v>180.23000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>